<commit_message>
feat(penjualan): add CRUD functionality with detail penjualan
</commit_message>
<xml_diff>
--- a/PWL_POS/public/template_penjualan.xlsx
+++ b/PWL_POS/public/template_penjualan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\= KULIAH\SEMESTER 4\3. PRAK JOBSHEET\PWL25\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F094B52F-597A-4BB9-9409-5AEF0E1A8D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AD6A92-0B23-437C-806B-50F13567B133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A7E97B80-A418-492F-A732-970E08D29917}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="10920" xr2:uid="{A7E97B80-A418-492F-A732-970E08D29917}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>user_id</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>PNJ-021</t>
+  </si>
+  <si>
+    <t>barang_id</t>
+  </si>
+  <si>
+    <t>jumlah</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -106,12 +115,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE8EE6D-4B72-42E2-BFD1-A7CC2131E7D3}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,9 +467,10 @@
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -472,8 +483,17 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>32</v>
       </c>
@@ -486,8 +506,17 @@
       <c r="D2" s="1">
         <v>45760</v>
       </c>
+      <c r="E2">
+        <v>27</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>950000</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>32</v>
       </c>
@@ -500,9 +529,27 @@
       <c r="D3" s="1">
         <v>45760</v>
       </c>
+      <c r="E3">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>10000</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>8000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix(stok, penjualan): change timeformat
</commit_message>
<xml_diff>
--- a/PWL_POS/public/template_penjualan.xlsx
+++ b/PWL_POS/public/template_penjualan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\= KULIAH\SEMESTER 4\3. PRAK JOBSHEET\PWL25\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AD6A92-0B23-437C-806B-50F13567B133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A341F209-6C7B-4118-A6AF-25338C60C4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="10920" xr2:uid="{A7E97B80-A418-492F-A732-970E08D29917}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A7E97B80-A418-492F-A732-970E08D29917}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>user_id</t>
   </si>
@@ -47,9 +47,6 @@
     <t>pembeli</t>
   </si>
   <si>
-    <t>penjualan_tanggal</t>
-  </si>
-  <si>
     <t>Ega Rivaldo</t>
   </si>
   <si>
@@ -66,18 +63,12 @@
   </si>
   <si>
     <t>jumlah</t>
-  </si>
-  <si>
-    <t>total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,9 +106,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,7 +449,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,49 +461,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>45760</v>
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>27</v>
       </c>
       <c r="E2">
-        <v>27</v>
-      </c>
-      <c r="F2">
         <v>1</v>
-      </c>
-      <c r="G2">
-        <v>950000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -521,34 +500,24 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>45760</v>
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>29</v>
       </c>
       <c r="E3">
-        <v>29</v>
-      </c>
-      <c r="F3">
         <v>1</v>
-      </c>
-      <c r="G3">
-        <v>10000</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
+      <c r="D4">
+        <v>30</v>
+      </c>
       <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="F4">
         <v>2</v>
-      </c>
-      <c r="G4">
-        <v>8000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>